<commit_message>
fixes for checkin template and jxls3 non-beta
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/checkin/Check-in_LETTER.xlsx
+++ b/owlcms/src/main/resources/templates/checkin/Check-in_LETTER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\checkin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B2E962-F91E-4092-97D2-4180B9E0D78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E9C8EB-1626-43D9-933B-4F12A25DA689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="1845" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2445" yWindow="3120" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start List" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:if(condition="session.description != null &amp;&amp; session.description != '' " lastCell="I10")</t>
+jx:if(condition="session.description != null &amp;&amp; session.description != '' " lastCell="I9")</t>
         </r>
       </text>
     </comment>
@@ -168,7 +168,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="session.athletes" var="l" varIndex="lIndex" orderBy="l.lastName ASC,l.firstName ASC" lastCell="I10")</t>
+jx:each(items="session.alphaAthletes" var="l" varIndex="lIndex" lastCell="I10")</t>
         </r>
       </text>
     </comment>
@@ -260,16 +260,16 @@
     <t>${lIndex + 1}</t>
   </si>
   <si>
+    <t>${session.weighInShortDateTime != "" ? (t.get("WeighInTime_StartList")+': '+session.weighInShortDateTime) : ""}      ${session.competitionShortDateTime != "" ? (t.get("StartTime_StartList")+': '+session.competitionShortDateTime) : ""}</t>
+  </si>
+  <si>
+    <t>${t.get("Preparation.Check-in")}</t>
+  </si>
+  <si>
+    <t>${ session.description }</t>
+  </si>
+  <si>
     <t>${t.get("Group")} ${session.name}</t>
-  </si>
-  <si>
-    <t>${ session.description }</t>
-  </si>
-  <si>
-    <t>${session.weighInShortDateTime != "" ? (t.get("WeighInTime_StartList")+': '+session.weighInShortDateTime) : ""}      ${session.competitionShortDateTime != "" ? (t.get("StartTime_StartList")+': '+session.competitionShortDateTime) : ""}</t>
-  </si>
-  <si>
-    <t>${t.get("Preparation.Check-in")}</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="8" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
@@ -1188,12 +1188,12 @@
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>

</xml_diff>